<commit_message>
Created dimentions, made configuration changes
</commit_message>
<xml_diff>
--- a/EDA/data_profiling.xlsx
+++ b/EDA/data_profiling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shivam_Bhongade\Desktop\practice\assesment\sales_data_modelling\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1886DCD1-2B60-4D8C-AB32-634D42818C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D847FB-01EB-4B20-8721-B3D2C90B1045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>column_name</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>38.03</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>only one order_id for multiple rows with different ASIN, amount</t>
   </si>
 </sst>
 </file>
@@ -186,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +217,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -235,11 +247,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -248,6 +271,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,9 +594,10 @@
     <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,8 +622,11 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -624,11 +655,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C3">
@@ -652,8 +683,11 @@
       <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -682,7 +716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -711,7 +745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -740,7 +774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -769,7 +803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -798,7 +832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -827,7 +861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -856,7 +890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -885,7 +919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -914,7 +948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -943,7 +977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -972,7 +1006,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1001,7 +1035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>

</xml_diff>